<commit_message>
Added test data files
</commit_message>
<xml_diff>
--- a/Deliverable 6/Final System Testing report.xlsx
+++ b/Deliverable 6/Final System Testing report.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mo\Documents\GitHub\Pizza\Deliverable 4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="12915" windowHeight="7245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12920" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="Defect_Serverity">Sheet2!$A$1:$A$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="51">
   <si>
     <t>Date Tested</t>
   </si>
@@ -266,7 +271,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,18 +552,18 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="18.90625" style="8" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" customWidth="1"/>
+    <col min="8" max="8" width="10.08984375" customWidth="1"/>
+    <col min="9" max="9" width="20.08984375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -590,7 +595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
@@ -611,7 +616,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -632,7 +637,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -653,7 +658,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
@@ -669,12 +674,16 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="I5" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
@@ -695,7 +704,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -711,12 +720,16 @@
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="I7" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -737,7 +750,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
@@ -758,7 +771,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
@@ -779,7 +792,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
@@ -800,7 +813,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
@@ -820,7 +833,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
@@ -845,7 +858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
@@ -866,7 +879,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
@@ -889,7 +902,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
@@ -910,7 +923,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
@@ -935,7 +948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>25</v>
       </c>
@@ -956,7 +969,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
@@ -977,7 +990,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
@@ -998,7 +1011,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
@@ -1019,7 +1032,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>27</v>
       </c>
@@ -1040,7 +1053,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -1061,7 +1074,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -1082,7 +1095,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
@@ -1103,7 +1116,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
@@ -1124,7 +1137,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
@@ -1145,7 +1158,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>30</v>
       </c>
@@ -1166,7 +1179,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>30</v>
       </c>
@@ -1187,7 +1200,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>31</v>
       </c>
@@ -1208,7 +1221,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>31</v>
       </c>
@@ -1229,7 +1242,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>33</v>
       </c>
@@ -1250,7 +1263,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>33</v>
       </c>
@@ -1271,7 +1284,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>32</v>
       </c>
@@ -1292,7 +1305,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>32</v>
       </c>
@@ -1313,7 +1326,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>34</v>
       </c>
@@ -1334,7 +1347,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>34</v>
       </c>
@@ -1355,7 +1368,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>35</v>
       </c>
@@ -1376,7 +1389,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>35</v>
       </c>
@@ -1397,7 +1410,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>36</v>
       </c>
@@ -1418,7 +1431,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>36</v>
       </c>
@@ -1439,7 +1452,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>37</v>
       </c>
@@ -1460,7 +1473,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>37</v>
       </c>
@@ -1481,7 +1494,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>38</v>
       </c>
@@ -1506,7 +1519,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>38</v>
       </c>
@@ -1531,7 +1544,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>39</v>
       </c>
@@ -1556,7 +1569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>39</v>
       </c>
@@ -1581,7 +1594,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>40</v>
       </c>
@@ -1602,7 +1615,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>40</v>
       </c>
@@ -1627,7 +1640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>41</v>
       </c>
@@ -1648,7 +1661,7 @@
       <c r="H50" s="3"/>
       <c r="I50" s="9"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>41</v>
       </c>
@@ -1692,7 +1705,7 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>